<commit_message>
new scenarios and reporting
</commit_message>
<xml_diff>
--- a/GlobalConfig/Global_configFile.xlsx
+++ b/GlobalConfig/Global_configFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Projects\POM_Framework\GlobalConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Projects\POM_framework\POM_Framework_mavenBuild\GlobalConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F655C02-BECF-4FDF-BEB1-4A6E1A80AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8F69D5-440C-48C4-8B9C-34D40A735110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -36,22 +36,19 @@
     <t>ApplicationUrl</t>
   </si>
   <si>
-    <t>wait.low</t>
-  </si>
-  <si>
-    <t>wait.medium</t>
-  </si>
-  <si>
-    <t>wait.high</t>
-  </si>
-  <si>
-    <t>wait.VrLow</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>https://courses.ultimateqa.com/users/sign_in</t>
+    <t>https://demo.guru99.com/test/newtours/</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>DemoUser1</t>
+  </si>
+  <si>
+    <t>VGVzdFVzZXJAMTIzNDU=</t>
   </si>
 </sst>
 </file>
@@ -102,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +109,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +396,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,48 +418,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>10</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>30</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>60</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>